<commit_message>
add Test Case for JobPlan source
</commit_message>
<xml_diff>
--- a/Integration Services Project/mapping/testcases-05-misc-v2.xlsx
+++ b/Integration Services Project/mapping/testcases-05-misc-v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\My Drive\2023-ste-coswinmigration\02-Project Execution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\STE.2022.CoswinMigration_2\Integration Services Project\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09F83BA-57A1-446E-B90B-6F3DD184881F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB853F0-D2A9-4719-BB0C-505482AD26B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="12" xr2:uid="{191A4E87-4E9E-45B3-AE4C-F999FE531A5D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="2" activeTab="10" xr2:uid="{191A4E87-4E9E-45B3-AE4C-F999FE531A5D}"/>
   </bookViews>
   <sheets>
     <sheet name="0501" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="179">
   <si>
     <t>#</t>
   </si>
@@ -2464,6 +2464,132 @@
   </si>
   <si>
     <t>JOBMATERIAL</t>
+  </si>
+  <si>
+    <t>Total migrated (JOB_DIR)</t>
+  </si>
+  <si>
+    <t>Sample data comparison (JOB_DIR)</t>
+  </si>
+  <si>
+    <t>Total migrated (EQP_JOBS)</t>
+  </si>
+  <si>
+    <t>Sample data comparison (EQP_JOBS)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Check the log table "ste_migration_log_details" (event = JOBPLAN, package_name = 0511_Misc_JobPlan_JPAssetsPLink_JobTask)
+Run the following SQL in coswindb:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>select count(*) FROM coswin.EQP_JOBS ej ;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pick sampling data by executing the following SQL in maximodb:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>select top 5 * from JOBPLAN where STE_MIGRATIONID is not null;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Take note the value of STE_MIGRATIONID
+Run the following SQL in coswindb:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SELECT 
+	ej.PK_EQP_JOBS 
+	, ej.EJ_JOB_ID 
+	, jd.JD_JOB_DS 	
+	, ej.EJ_DURN 
+	, ej.EJ_DU_UNIT
+	, CASE WHEN ej.EJ_DU_UNIT=87 THEN ej.EJ_DURN * 7 * 24
+	       WHEN ej.EJ_DU_UNIT=68 THEN ej.EJ_DURN * 24
+	       ELSE ej.EJ_DURN 
+	  END AS JPDURATION
+	, CASE WHEN ej.EJ_DU_UNIT=87 THEN 'WEEKS'
+	       WHEN ej.EJ_DU_UNIT=68 THEN 'DAYS'
+	       ELSE 'HOURS'
+	  END AS DURATIONUNIT
+	, ej.EJ_PRIORITY 
+	, ej.EJ_SUPV 
+	, ej.EJ_LUDT 
+	, EJ_AVPRTM
+	, EJ_COSC
+	, EJ_DAY
+	, EJ_ENWK
+	, EJ_HAZARD
+	, EJ_JBBHU
+	, EJ_JBCLU
+	, EJ_JBTYU
+	, EJ_LAB_SCOST
+	, EJ_LJML
+	, EJ_MAT_SCOST
+	, EJ_MIPRTM
+	, EJ_MTID
+	, EJ_MTPRML
+	, EJ_MXPRTM
+	, EJ_NOWO
+	, EJ_PR_UNIT
+	, EJ_PRJ_REF
+	, EJ_FM_COST
+	, EJ_STWK
+	, EJ_WOID
+	, EJ_WORK_DAYS
+	, EJ_WP_TYPE
+	, et.EQ_EQCD
+FROM COSWIN.EQP_JOBS ej 
+LEFT JOIN COSWIN.JOB_DIR jd ON jd.PK_JOB_DIR = ej.JD_EJ_18 
+LEFT JOIN COSWIN.EQP_TOPO et ON et.PK_EQP_TOPO = ej.EQ_EJ_17
+where ej.PK_EQO_JOBS in (x)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+(x is the previously noted STE_MIGRATIONID)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3137,7 +3263,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G4" sqref="G4"/>
       <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
@@ -3373,12 +3499,12 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC8E1932-F171-4A4B-B66A-AB2698403602}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G4" sqref="G4"/>
-      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3438,7 +3564,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="7" t="str">
-        <f t="shared" ref="E2:E20" si="0">CONCATENATE(C2,"-",A2)</f>
+        <f t="shared" ref="E2:E22" si="0">CONCATENATE(C2,"-",A2)</f>
         <v>0511-1</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -3475,7 +3601,7 @@
         <v>14</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>145</v>
@@ -3505,7 +3631,7 @@
         <v>14</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>17</v>
+        <v>174</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>146</v>
@@ -3514,7 +3640,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -3528,23 +3654,23 @@
         <v>66</v>
       </c>
       <c r="E5" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E5:E6" si="1">CONCATENATE(C5,"-",A5)</f>
         <v>0511-4</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>147</v>
+        <v>177</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -3558,25 +3684,25 @@
         <v>66</v>
       </c>
       <c r="E6" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0511-5</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>70</v>
+        <v>176</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>178</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>31</v>
@@ -3589,24 +3715,24 @@
       </c>
       <c r="E7" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>0511-6</v>
+        <v>0511-4</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>147</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>31</v>
@@ -3619,24 +3745,24 @@
       </c>
       <c r="E8" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>0511-7</v>
+        <v>0511-5</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>21</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>31</v>
@@ -3645,28 +3771,28 @@
         <v>92</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E9" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>0511-8</v>
+        <v>0511-6</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>148</v>
+        <v>24</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" customFormat="1" ht="345" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>31</v>
@@ -3675,28 +3801,28 @@
         <v>92</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>0511-9</v>
+        <v>0511-7</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>149</v>
+        <v>27</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>31</v>
@@ -3709,24 +3835,24 @@
       </c>
       <c r="E11" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>0511-10</v>
+        <v>0511-8</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" customFormat="1" ht="345" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>31</v>
@@ -3739,24 +3865,24 @@
       </c>
       <c r="E12" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>0511-11</v>
+        <v>0511-9</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>74</v>
+        <v>17</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>149</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>31</v>
@@ -3769,24 +3895,24 @@
       </c>
       <c r="E13" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>0511-12</v>
+        <v>0511-10</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>150</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>31</v>
@@ -3799,24 +3925,24 @@
       </c>
       <c r="E14" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>0511-13</v>
+        <v>0511-11</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>21</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>31</v>
@@ -3825,28 +3951,28 @@
         <v>92</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E15" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>0511-14</v>
+        <v>0511-12</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>142</v>
+        <v>24</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>31</v>
@@ -3855,28 +3981,28 @@
         <v>92</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E16" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>0511-15</v>
+        <v>0511-13</v>
       </c>
       <c r="F16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
         <v>14</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>31</v>
@@ -3889,24 +4015,24 @@
       </c>
       <c r="E17" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>0511-16</v>
+        <v>0511-14</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>31</v>
@@ -3919,24 +4045,24 @@
       </c>
       <c r="E18" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>0511-17</v>
+        <v>0511-15</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>73</v>
+        <v>17</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>143</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>31</v>
@@ -3949,24 +4075,24 @@
       </c>
       <c r="E19" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>0511-18</v>
+        <v>0511-16</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>144</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>31</v>
@@ -3979,18 +4105,78 @@
       </c>
       <c r="E20" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>0511-19</v>
+        <v>0511-17</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>21</v>
       </c>
       <c r="G20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>18</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0511-18</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>19</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0511-19</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="H22" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="I22" s="8" t="s">
         <v>29</v>
       </c>
     </row>
@@ -4005,7 +4191,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G8" sqref="G8"/>
       <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
@@ -4273,8 +4459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE37274C-5E3F-4893-9FC8-D055E01C3B35}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G8" sqref="G8"/>
       <selection pane="bottomLeft" activeCell="D4" sqref="D4:D8"/>
     </sheetView>
@@ -6730,7 +6916,7 @@
     <sheetView topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G8" sqref="G8"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6997,7 +7183,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G8" sqref="G8"/>
       <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
@@ -7565,7 +7751,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G8" sqref="G8"/>
       <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>

</xml_diff>